<commit_message>
Renaming results files and adding new results
</commit_message>
<xml_diff>
--- a/results/epsilon/tictactoe/normal/TicTacToeNormal_EpsilonResults_Wins_Comparison.xlsx
+++ b/results/epsilon/tictactoe/normal/TicTacToeNormal_EpsilonResults_Wins_Comparison.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="TicTacToeNormal_EpsilonResults_" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Epsilon</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>320k</t>
+  </si>
+  <si>
+    <t>640k</t>
   </si>
 </sst>
 </file>
@@ -3999,6 +4002,337 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TicTacToeNormal_EpsilonResults_!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>640k</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>TicTacToeNormal_EpsilonResults_!$H$2:$H$102</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0.39037500000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.70390937499999995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.68436562499999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.705175</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.70777968749999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69985468750000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.71032499999999998</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.70073437500000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69468593749999996</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.68960468750000004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.70449218749999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.6902390625</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.68257500000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.68611406249999995</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.68248750000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.68361562499999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.68430781249999995</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.67770624999999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.68733124999999995</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.66830468750000005</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.68865781250000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.67340937499999998</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.67721562499999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.66316093750000005</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.66660624999999996</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.66702343750000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.66502343750000004</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.66292343750000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.67176718749999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.65680781249999998</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.6496046875</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.64999375000000004</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.65229062500000001</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.65481093749999997</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.64938437500000001</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.64366093749999997</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.64211249999999997</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.64134374999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.63447968749999994</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.63262031249999995</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.636003125</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.63506249999999997</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.63156406249999997</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.6282171875</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.62640781249999999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.62325937499999995</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.61982031250000003</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.62097500000000005</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.61435625000000005</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.61191718750000001</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.61088437500000003</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.60671562499999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.60308437500000001</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.60032968750000004</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.59822187500000001</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.59655781249999995</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.59125156249999999</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.59160468749999995</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.58879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.58154375000000003</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.58128281250000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.57852187499999996</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.57572343749999999</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.57180781250000001</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.56848281249999999</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.567071875</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.56093906250000003</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.55994218750000002</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.55700468749999998</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.55146406250000002</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.54985312500000005</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.54758906249999995</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.54297343750000004</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.53953437500000001</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.53582031249999995</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.53228281249999998</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.52888593750000001</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.526246875</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.52189375000000005</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.51715468750000004</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.51478906250000001</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.51148593750000004</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.50629531250000004</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.50388906249999998</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.49956093750000002</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.49552499999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.49235781249999999</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.48850937500000002</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.48502187499999999</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.481565625</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.47592968749999998</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>0.47396874999999999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>0.46903281250000001</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.46468437499999998</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>0.4611515625</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>0.4565796875</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>0.45249531250000002</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>0.44873437500000002</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>0.44478593750000001</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.44148749999999998</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.436596875</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -4009,11 +4343,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="199542656"/>
-        <c:axId val="199613824"/>
+        <c:axId val="224996352"/>
+        <c:axId val="225019008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="199542656"/>
+        <c:axId val="224996352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4042,7 +4376,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199613824"/>
+        <c:crossAx val="225019008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4052,7 +4386,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="199613824"/>
+        <c:axId val="225019008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4083,7 +4417,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="199542656"/>
+        <c:crossAx val="224996352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4429,18 +4763,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G102"/>
+  <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="7" width="8.7265625" style="1"/>
+    <col min="2" max="8" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4462,8 +4796,11 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -4485,8 +4822,11 @@
       <c r="G2" s="1">
         <v>0.377928125</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H2" s="1">
+        <v>0.39037500000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.01</v>
       </c>
@@ -4508,8 +4848,11 @@
       <c r="G3" s="1">
         <v>0.61886562499999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H3" s="1">
+        <v>0.70390937499999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.02</v>
       </c>
@@ -4531,8 +4874,11 @@
       <c r="G4" s="1">
         <v>0.66978749999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H4" s="1">
+        <v>0.68436562499999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.03</v>
       </c>
@@ -4554,8 +4900,11 @@
       <c r="G5" s="1">
         <v>0.68322812499999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H5" s="1">
+        <v>0.705175</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.04</v>
       </c>
@@ -4577,8 +4926,11 @@
       <c r="G6" s="1">
         <v>0.70002187500000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H6" s="1">
+        <v>0.70777968749999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.05</v>
       </c>
@@ -4600,8 +4952,11 @@
       <c r="G7" s="1">
         <v>0.68030625</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H7" s="1">
+        <v>0.69985468750000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.06</v>
       </c>
@@ -4623,8 +4978,11 @@
       <c r="G8" s="1">
         <v>0.68581562500000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H8" s="1">
+        <v>0.71032499999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4646,8 +5004,11 @@
       <c r="G9" s="1">
         <v>0.68230625</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H9" s="1">
+        <v>0.70073437500000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.08</v>
       </c>
@@ -4669,8 +5030,11 @@
       <c r="G10" s="1">
         <v>0.70042812499999996</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H10" s="1">
+        <v>0.69468593749999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.09</v>
       </c>
@@ -4692,8 +5056,11 @@
       <c r="G11" s="1">
         <v>0.688165625</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H11" s="1">
+        <v>0.68960468750000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9.9999999999999895E-2</v>
       </c>
@@ -4715,8 +5082,11 @@
       <c r="G12" s="1">
         <v>0.68220312500000002</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H12" s="1">
+        <v>0.70449218749999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.109999999999999</v>
       </c>
@@ -4738,8 +5108,11 @@
       <c r="G13" s="1">
         <v>0.66898749999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H13" s="1">
+        <v>0.6902390625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.119999999999999</v>
       </c>
@@ -4761,8 +5134,11 @@
       <c r="G14" s="1">
         <v>0.68130937499999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H14" s="1">
+        <v>0.68257500000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.12999999999999901</v>
       </c>
@@ -4784,8 +5160,11 @@
       <c r="G15" s="1">
         <v>0.68158437500000002</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H15" s="1">
+        <v>0.68611406249999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.13999999999999899</v>
       </c>
@@ -4807,8 +5186,11 @@
       <c r="G16" s="1">
         <v>0.67464687499999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H16" s="1">
+        <v>0.68248750000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.15</v>
       </c>
@@ -4830,8 +5212,11 @@
       <c r="G17" s="1">
         <v>0.67020625</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="1">
+        <v>0.68361562499999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.16</v>
       </c>
@@ -4853,8 +5238,11 @@
       <c r="G18" s="1">
         <v>0.66353437500000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H18" s="1">
+        <v>0.68430781249999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.17</v>
       </c>
@@ -4876,8 +5264,11 @@
       <c r="G19" s="1">
         <v>0.66497499999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H19" s="1">
+        <v>0.67770624999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.18</v>
       </c>
@@ -4899,8 +5290,11 @@
       <c r="G20" s="1">
         <v>0.68352187499999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H20" s="1">
+        <v>0.68733124999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.19</v>
       </c>
@@ -4922,8 +5316,11 @@
       <c r="G21" s="1">
         <v>0.67250312499999998</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H21" s="1">
+        <v>0.66830468750000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.2</v>
       </c>
@@ -4945,8 +5342,11 @@
       <c r="G22" s="1">
         <v>0.67602499999999999</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H22" s="1">
+        <v>0.68865781250000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.21</v>
       </c>
@@ -4968,8 +5368,11 @@
       <c r="G23" s="1">
         <v>0.65962187500000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H23" s="1">
+        <v>0.67340937499999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.22</v>
       </c>
@@ -4991,8 +5394,11 @@
       <c r="G24" s="1">
         <v>0.66231249999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H24" s="1">
+        <v>0.67721562499999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.23</v>
       </c>
@@ -5014,8 +5420,11 @@
       <c r="G25" s="1">
         <v>0.66413437500000005</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H25" s="1">
+        <v>0.66316093750000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.24</v>
       </c>
@@ -5037,8 +5446,11 @@
       <c r="G26" s="1">
         <v>0.65947500000000003</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H26" s="1">
+        <v>0.66660624999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.25</v>
       </c>
@@ -5060,8 +5472,11 @@
       <c r="G27" s="1">
         <v>0.65684374999999995</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H27" s="1">
+        <v>0.66702343750000004</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.26</v>
       </c>
@@ -5083,8 +5498,11 @@
       <c r="G28" s="1">
         <v>0.64971250000000003</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H28" s="1">
+        <v>0.66502343750000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.27</v>
       </c>
@@ -5106,8 +5524,11 @@
       <c r="G29" s="1">
         <v>0.65945937499999996</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H29" s="1">
+        <v>0.66292343750000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.28000000000000003</v>
       </c>
@@ -5129,8 +5550,11 @@
       <c r="G30" s="1">
         <v>0.65440312499999997</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H30" s="1">
+        <v>0.67176718749999997</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.28999999999999998</v>
       </c>
@@ -5152,8 +5576,11 @@
       <c r="G31" s="1">
         <v>0.64801874999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H31" s="1">
+        <v>0.65680781249999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.3</v>
       </c>
@@ -5175,8 +5602,11 @@
       <c r="G32" s="1">
         <v>0.65247500000000003</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H32" s="1">
+        <v>0.6496046875</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.31</v>
       </c>
@@ -5198,8 +5628,11 @@
       <c r="G33" s="1">
         <v>0.64831875000000005</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H33" s="1">
+        <v>0.64999375000000004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.32</v>
       </c>
@@ -5221,8 +5654,11 @@
       <c r="G34" s="1">
         <v>0.64302187499999997</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H34" s="1">
+        <v>0.65229062500000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.33</v>
       </c>
@@ -5244,8 +5680,11 @@
       <c r="G35" s="1">
         <v>0.64342500000000002</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H35" s="1">
+        <v>0.65481093749999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.34</v>
       </c>
@@ -5267,8 +5706,11 @@
       <c r="G36" s="1">
         <v>0.64435312499999997</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H36" s="1">
+        <v>0.64938437500000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.35</v>
       </c>
@@ -5290,8 +5732,11 @@
       <c r="G37" s="1">
         <v>0.643865625</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H37" s="1">
+        <v>0.64366093749999997</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.36</v>
       </c>
@@ -5313,8 +5758,11 @@
       <c r="G38" s="1">
         <v>0.63898437500000005</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H38" s="1">
+        <v>0.64211249999999997</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.37</v>
       </c>
@@ -5336,8 +5784,11 @@
       <c r="G39" s="1">
         <v>0.632528125</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H39" s="1">
+        <v>0.64134374999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.38</v>
       </c>
@@ -5359,8 +5810,11 @@
       <c r="G40" s="1">
         <v>0.62994687500000002</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H40" s="1">
+        <v>0.63447968749999994</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.39</v>
       </c>
@@ -5382,8 +5836,11 @@
       <c r="G41" s="1">
         <v>0.63364374999999995</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H41" s="1">
+        <v>0.63262031249999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.4</v>
       </c>
@@ -5405,8 +5862,11 @@
       <c r="G42" s="1">
         <v>0.62956562500000002</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H42" s="1">
+        <v>0.636003125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.41</v>
       </c>
@@ -5428,8 +5888,11 @@
       <c r="G43" s="1">
         <v>0.62638749999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H43" s="1">
+        <v>0.63506249999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.42</v>
       </c>
@@ -5451,8 +5914,11 @@
       <c r="G44" s="1">
         <v>0.62255312500000004</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H44" s="1">
+        <v>0.63156406249999997</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.43</v>
       </c>
@@ -5474,8 +5940,11 @@
       <c r="G45" s="1">
         <v>0.62395</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H45" s="1">
+        <v>0.6282171875</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.44</v>
       </c>
@@ -5497,8 +5966,11 @@
       <c r="G46" s="1">
         <v>0.61688750000000003</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H46" s="1">
+        <v>0.62640781249999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.45</v>
       </c>
@@ -5520,8 +5992,11 @@
       <c r="G47" s="1">
         <v>0.61762187499999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H47" s="1">
+        <v>0.62325937499999995</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.46</v>
       </c>
@@ -5543,8 +6018,11 @@
       <c r="G48" s="1">
         <v>0.61495937499999997</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H48" s="1">
+        <v>0.61982031250000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.47</v>
       </c>
@@ -5566,8 +6044,11 @@
       <c r="G49" s="1">
         <v>0.61180000000000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H49" s="1">
+        <v>0.62097500000000005</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.48</v>
       </c>
@@ -5589,8 +6070,11 @@
       <c r="G50" s="1">
         <v>0.60653437499999996</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H50" s="1">
+        <v>0.61435625000000005</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.49</v>
       </c>
@@ -5612,8 +6096,11 @@
       <c r="G51" s="1">
         <v>0.61038749999999997</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H51" s="1">
+        <v>0.61191718750000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.5</v>
       </c>
@@ -5635,8 +6122,11 @@
       <c r="G52" s="1">
         <v>0.60013749999999999</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H52" s="1">
+        <v>0.61088437500000003</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.51</v>
       </c>
@@ -5658,8 +6148,11 @@
       <c r="G53" s="1">
         <v>0.59984999999999999</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H53" s="1">
+        <v>0.60671562499999998</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.52</v>
       </c>
@@ -5681,8 +6174,11 @@
       <c r="G54" s="1">
         <v>0.598321875</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H54" s="1">
+        <v>0.60308437500000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.53</v>
       </c>
@@ -5704,8 +6200,11 @@
       <c r="G55" s="1">
         <v>0.59637812499999998</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H55" s="1">
+        <v>0.60032968750000004</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.54</v>
       </c>
@@ -5727,8 +6226,11 @@
       <c r="G56" s="1">
         <v>0.593846875</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H56" s="1">
+        <v>0.59822187500000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.55000000000000004</v>
       </c>
@@ -5750,8 +6252,11 @@
       <c r="G57" s="1">
         <v>0.58986875000000005</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H57" s="1">
+        <v>0.59655781249999995</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>0.56000000000000005</v>
       </c>
@@ -5773,8 +6278,11 @@
       <c r="G58" s="1">
         <v>0.58748437499999995</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H58" s="1">
+        <v>0.59125156249999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.56999999999999995</v>
       </c>
@@ -5796,8 +6304,11 @@
       <c r="G59" s="1">
         <v>0.58537187499999999</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H59" s="1">
+        <v>0.59160468749999995</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.57999999999999996</v>
       </c>
@@ -5819,8 +6330,11 @@
       <c r="G60" s="1">
         <v>0.58446874999999998</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H60" s="1">
+        <v>0.58879999999999999</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.59</v>
       </c>
@@ -5842,8 +6356,11 @@
       <c r="G61" s="1">
         <v>0.58080937499999996</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H61" s="1">
+        <v>0.58154375000000003</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.6</v>
       </c>
@@ -5865,8 +6382,11 @@
       <c r="G62" s="1">
         <v>0.57584687499999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H62" s="1">
+        <v>0.58128281250000002</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>0.61</v>
       </c>
@@ -5888,8 +6408,11 @@
       <c r="G63" s="1">
         <v>0.57567500000000005</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H63" s="1">
+        <v>0.57852187499999996</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>0.62</v>
       </c>
@@ -5911,8 +6434,11 @@
       <c r="G64" s="1">
         <v>0.57014687500000005</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H64" s="1">
+        <v>0.57572343749999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>0.63</v>
       </c>
@@ -5934,8 +6460,11 @@
       <c r="G65" s="1">
         <v>0.57017187499999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H65" s="1">
+        <v>0.57180781250000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>0.64</v>
       </c>
@@ -5957,8 +6486,11 @@
       <c r="G66" s="1">
         <v>0.56461249999999996</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H66" s="1">
+        <v>0.56848281249999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>0.65</v>
       </c>
@@ -5980,8 +6512,11 @@
       <c r="G67" s="1">
         <v>0.56240625</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H67" s="1">
+        <v>0.567071875</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>0.66</v>
       </c>
@@ -6003,8 +6538,11 @@
       <c r="G68" s="1">
         <v>0.56016250000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H68" s="1">
+        <v>0.56093906250000003</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>0.67</v>
       </c>
@@ -6026,8 +6564,11 @@
       <c r="G69" s="1">
         <v>0.55641874999999996</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H69" s="1">
+        <v>0.55994218750000002</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>0.68</v>
       </c>
@@ -6049,8 +6590,11 @@
       <c r="G70" s="1">
         <v>0.55278437499999999</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H70" s="1">
+        <v>0.55700468749999998</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.69</v>
       </c>
@@ -6072,8 +6616,11 @@
       <c r="G71" s="1">
         <v>0.55057187500000004</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H71" s="1">
+        <v>0.55146406250000002</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>0.7</v>
       </c>
@@ -6095,8 +6642,11 @@
       <c r="G72" s="1">
         <v>0.54835624999999999</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H72" s="1">
+        <v>0.54985312500000005</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>0.71</v>
       </c>
@@ -6118,8 +6668,11 @@
       <c r="G73" s="1">
         <v>0.54227499999999995</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H73" s="1">
+        <v>0.54758906249999995</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0.72</v>
       </c>
@@ -6141,8 +6694,11 @@
       <c r="G74" s="1">
         <v>0.53953437500000001</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H74" s="1">
+        <v>0.54297343750000004</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>0.73</v>
       </c>
@@ -6164,8 +6720,11 @@
       <c r="G75" s="1">
         <v>0.53709687500000003</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H75" s="1">
+        <v>0.53953437500000001</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.74</v>
       </c>
@@ -6187,8 +6746,11 @@
       <c r="G76" s="1">
         <v>0.53516249999999999</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H76" s="1">
+        <v>0.53582031249999995</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>0.75</v>
       </c>
@@ -6210,8 +6772,11 @@
       <c r="G77" s="1">
         <v>0.53125624999999999</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H77" s="1">
+        <v>0.53228281249999998</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>0.76</v>
       </c>
@@ -6233,8 +6798,11 @@
       <c r="G78" s="1">
         <v>0.52797499999999997</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H78" s="1">
+        <v>0.52888593750000001</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>0.77</v>
       </c>
@@ -6256,8 +6824,11 @@
       <c r="G79" s="1">
         <v>0.52423125000000004</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H79" s="1">
+        <v>0.526246875</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>0.78</v>
       </c>
@@ -6279,8 +6850,11 @@
       <c r="G80" s="1">
         <v>0.51951875000000003</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80" s="1">
+        <v>0.52189375000000005</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>0.79</v>
       </c>
@@ -6302,8 +6876,11 @@
       <c r="G81" s="1">
         <v>0.51621562499999996</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H81" s="1">
+        <v>0.51715468750000004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>0.8</v>
       </c>
@@ -6325,8 +6902,11 @@
       <c r="G82" s="1">
         <v>0.51297812499999995</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" s="1">
+        <v>0.51478906250000001</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.81</v>
       </c>
@@ -6348,8 +6928,11 @@
       <c r="G83" s="1">
         <v>0.50725937499999996</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H83" s="1">
+        <v>0.51148593750000004</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>0.82</v>
       </c>
@@ -6371,8 +6954,11 @@
       <c r="G84" s="1">
         <v>0.50360000000000005</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H84" s="1">
+        <v>0.50629531250000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>0.83</v>
       </c>
@@ -6394,8 +6980,11 @@
       <c r="G85" s="1">
         <v>0.502809375</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H85" s="1">
+        <v>0.50388906249999998</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>0.84</v>
       </c>
@@ -6417,8 +7006,11 @@
       <c r="G86" s="1">
         <v>0.497403125</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86" s="1">
+        <v>0.49956093750000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>0.85</v>
       </c>
@@ -6440,8 +7032,11 @@
       <c r="G87" s="1">
         <v>0.49581874999999997</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87" s="1">
+        <v>0.49552499999999999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>0.86</v>
       </c>
@@ -6463,8 +7058,11 @@
       <c r="G88" s="1">
         <v>0.48985937499999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H88" s="1">
+        <v>0.49235781249999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>0.87</v>
       </c>
@@ -6486,8 +7084,11 @@
       <c r="G89" s="1">
         <v>0.48591875000000001</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89" s="1">
+        <v>0.48850937500000002</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>0.88</v>
       </c>
@@ -6509,8 +7110,11 @@
       <c r="G90" s="1">
         <v>0.48498124999999997</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" s="1">
+        <v>0.48502187499999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>0.89</v>
       </c>
@@ -6532,8 +7136,11 @@
       <c r="G91" s="1">
         <v>0.47898750000000001</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91" s="1">
+        <v>0.481565625</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.9</v>
       </c>
@@ -6555,8 +7162,11 @@
       <c r="G92" s="1">
         <v>0.47583437499999998</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92" s="1">
+        <v>0.47592968749999998</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>0.91</v>
       </c>
@@ -6578,8 +7188,11 @@
       <c r="G93" s="1">
         <v>0.47272187500000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93" s="1">
+        <v>0.47396874999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>0.92</v>
       </c>
@@ -6601,8 +7214,11 @@
       <c r="G94" s="1">
         <v>0.46681250000000002</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H94" s="1">
+        <v>0.46903281250000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>0.93</v>
       </c>
@@ -6624,8 +7240,11 @@
       <c r="G95" s="1">
         <v>0.46376250000000002</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H95" s="1">
+        <v>0.46468437499999998</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>0.94</v>
       </c>
@@ -6647,8 +7266,11 @@
       <c r="G96" s="1">
         <v>0.46053749999999999</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H96" s="1">
+        <v>0.4611515625</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>0.95</v>
       </c>
@@ -6670,8 +7292,11 @@
       <c r="G97" s="1">
         <v>0.45513124999999999</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H97" s="1">
+        <v>0.4565796875</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>0.96</v>
       </c>
@@ -6693,8 +7318,11 @@
       <c r="G98" s="1">
         <v>0.45221562500000001</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H98" s="1">
+        <v>0.45249531250000002</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>0.97</v>
       </c>
@@ -6716,8 +7344,11 @@
       <c r="G99" s="1">
         <v>0.44742187500000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H99" s="1">
+        <v>0.44873437500000002</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>0.98</v>
       </c>
@@ -6739,8 +7370,11 @@
       <c r="G100" s="1">
         <v>0.44425937500000001</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H100" s="1">
+        <v>0.44478593750000001</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>0.99</v>
       </c>
@@ -6762,8 +7396,11 @@
       <c r="G101" s="1">
         <v>0.44156250000000002</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H101" s="1">
+        <v>0.44148749999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1</v>
       </c>
@@ -6784,6 +7421,9 @@
       </c>
       <c r="G102" s="1">
         <v>0.43608437500000002</v>
+      </c>
+      <c r="H102" s="1">
+        <v>0.436596875</v>
       </c>
     </row>
   </sheetData>
@@ -6795,7 +7435,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>